<commit_message>
Local Excel Database Setup
</commit_message>
<xml_diff>
--- a/my_project/data/questions.xlsx
+++ b/my_project/data/questions.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agamp\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agamp\OneDrive\Documents\mocktest_backend\my_project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4C11542-EA03-4B04-BD96-34871DA1A2B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9B7372B-572A-4EC7-A650-C84D1F1C3FD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B1B2FAE3-7802-4EAC-AD39-5B9250518982}"/>
   </bookViews>
@@ -3328,7 +3328,7 @@
   <dimension ref="A1:E128"/>
   <sheetViews>
     <sheetView showRowColHeaders="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>